<commit_message>
CRITICAL - 交易程序发生异常: Index(['ID'], dtype='object')
</commit_message>
<xml_diff>
--- a/data/account_metrics.xlsx
+++ b/data/account_metrics.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F242"/>
+  <dimension ref="A1:F322"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7819,6 +7819,2452 @@
         </is>
       </c>
     </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>position_file</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>pos20250529_v3.csv</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>调仓文件</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:04:41</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>before_trade_balance</t>
+        </is>
+      </c>
+      <c r="B244" t="n">
+        <v>48.04205943</v>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>调仓前账户总保证金余额(totalMarginBalance)</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:04:41</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>before_available_balance</t>
+        </is>
+      </c>
+      <c r="B245" t="n">
+        <v>12.44484729</v>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>调仓前可用保证金余额(available_balance)</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:04:41</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>after_trade_balance</t>
+        </is>
+      </c>
+      <c r="B246" t="n">
+        <v>48.06005427</v>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>调仓后账户总保证金余额(totalMarginBalance)</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>balance_loss</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>-0.01799484000000007</v>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>调仓前后账户余额变化</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>balance_loss_rate</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>-0.037456%</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>调仓前后账户余额变化率(%)</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>after_available_balance</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>6.08346489</v>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>调仓后可用保证金余额(available_balance)</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>btc_usdt_price</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>107793.8</v>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>当前 BTC/USDT 价格: 107793.8</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>trade_commission_summary_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>0</v>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易手续费总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>trade_commission_summary_ratio_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>0</v>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易手续费总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>trade_realized_pnl_summary_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>0</v>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易已实现盈亏总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>trade_realized_pnl_summary_ratio_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>0</v>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易已实现盈亏总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>pre_rebalance_return</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>0.000000%</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>调仓前回报率: 无历史数据</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>post_rebalance_return</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>0.000000%</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>调仓后回报率: 无历史数据</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:06:38</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>2025-05-29_1504:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>position_file</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>pos20250529_v3.csv</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>调仓文件</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:07:39</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>before_trade_balance</t>
+        </is>
+      </c>
+      <c r="B258" t="n">
+        <v>48.03734973</v>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>调仓前账户总保证金余额(totalMarginBalance)</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:07:39</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>before_available_balance</t>
+        </is>
+      </c>
+      <c r="B259" t="n">
+        <v>6.06452259</v>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>调仓前可用保证金余额(available_balance)</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:07:39</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>after_trade_balance</t>
+        </is>
+      </c>
+      <c r="B260" t="n">
+        <v>48.06005427</v>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>调仓后账户总保证金余额(totalMarginBalance)</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>balance_loss</t>
+        </is>
+      </c>
+      <c r="B261" t="n">
+        <v>-0.02270453999999944</v>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>调仓前后账户余额变化</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:08:47</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>balance_loss_rate</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>-0.047264%</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>调仓前后账户余额变化率(%)</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:08:47</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>after_available_balance</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>6.08346489</v>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>调仓后可用保证金余额(available_balance)</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>btc_usdt_price</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>107793.8</v>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>当前 BTC/USDT 价格: 107793.8</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>trade_commission_summary_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>0</v>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易手续费总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>trade_commission_summary_ratio_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>0</v>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易手续费总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>trade_realized_pnl_summary_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>0</v>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易已实现盈亏总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>trade_realized_pnl_summary_ratio_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>0</v>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易已实现盈亏总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>pre_rebalance_return</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>0.000000%</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>调仓前回报率: 无历史数据</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:08:47</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>post_rebalance_return</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>0.000000%</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>调仓后回报率: 无历史数据</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:08:47</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:08:47</t>
+        </is>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>2025-05-29_1507:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>position_file</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>pos20250529_v3.csv</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>调仓文件</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:09:48</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>before_trade_balance</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>48.06883907</v>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>调仓前账户总保证金余额(totalMarginBalance)</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:09:48</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>before_available_balance</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>6.146924</v>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>调仓前可用保证金余额(available_balance)</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:09:48</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>after_trade_balance</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>48.06005427</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>调仓后账户总保证金余额(totalMarginBalance)</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>balance_loss</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>0.008784800000000814</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>调仓前后账户余额变化</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:10:53</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>balance_loss_rate</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>0.018275%</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>调仓前后账户余额变化率(%)</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:10:53</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>after_available_balance</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>6.08346489</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>调仓后可用保证金余额(available_balance)</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>btc_usdt_price</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>107793.8</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>当前 BTC/USDT 价格: 107793.8</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>trade_commission_summary_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>0</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易手续费总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>trade_commission_summary_ratio_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>0</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易手续费总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>trade_realized_pnl_summary_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>0</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易已实现盈亏总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>trade_realized_pnl_summary_ratio_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>0</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易已实现盈亏总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>pre_rebalance_return</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>0.000000%</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>调仓前回报率: 无历史数据</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:10:52</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>post_rebalance_return</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>0.000000%</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>调仓后回报率: 无历史数据</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:10:52</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:10:53</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>2025-05-29_1509:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>position_file</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>pos20250529_v3.csv</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>调仓文件</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:11:53</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>before_trade_balance</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>48.03375522</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>调仓前账户总保证金余额(totalMarginBalance)</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:11:53</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>before_available_balance</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>6.01584109</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>调仓前可用保证金余额(available_balance)</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:11:53</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>after_trade_balance</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>48.06005427</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>调仓后账户总保证金余额(totalMarginBalance)</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>balance_loss</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>-0.02629904999999866</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>调仓前后账户余额变化</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:13:07</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>balance_loss_rate</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>-0.054751%</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>调仓前后账户余额变化率(%)</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:13:07</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>after_available_balance</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>6.08346489</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>调仓后可用保证金余额(available_balance)</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>btc_usdt_price</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>107793.8</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>当前 BTC/USDT 价格: 107793.8</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>trade_commission_summary_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>0</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易手续费总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>trade_commission_summary_ratio_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>0</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易手续费总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>trade_realized_pnl_summary_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>0</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易已实现盈亏总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>trade_realized_pnl_summary_ratio_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>0</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易已实现盈亏总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:06:38</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>pre_rebalance_return</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>0.000000%</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>调仓前回报率: 无历史数据</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:13:07</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>post_rebalance_return</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>0.000000%</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>调仓后回报率: 无历史数据</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:13:07</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:13:07</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>2025-05-29_1511:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>position_file</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>pos20250529_v3.csv</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>调仓文件</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:32:16</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:32:16</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>2025-05-29_1532:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>after_trade_balance</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>48.07111186</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>调仓后账户总保证金余额(totalMarginBalance)</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:32:16</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:32:16</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>2025-05-29_1532:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>after_available_balance</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>6.01014839</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>调仓后可用保证金余额(available_balance)</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:32:16</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:32:16</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>2025-05-29_1532:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>btc_usdt_price</t>
+        </is>
+      </c>
+      <c r="B302" t="n">
+        <v>107899.7</v>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>当前 BTC/USDT 价格: 107899.7</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:32:16</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:32:16</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>2025-05-29_1532:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>trade_commission_summary_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B303" t="n">
+        <v>0</v>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易手续费总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:32:16</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:32:16</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>2025-05-29_1532:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>trade_commission_summary_ratio_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B304" t="n">
+        <v>0</v>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易手续费总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:32:16</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:32:16</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>2025-05-29_1532:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>trade_realized_pnl_summary_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
+        <v>0</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易已实现盈亏总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:32:16</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:32:16</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>2025-05-29_1532:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>trade_realized_pnl_summary_ratio_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B306" t="n">
+        <v>0</v>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易已实现盈亏总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:32:16</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:32:16</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>2025-05-29_1532:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>pre_rebalance_return</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>0.000000%</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>调仓前回报率: 首次运行或缺少历史数据</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:32:16</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:32:16</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>2025-05-29_1532:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>post_rebalance_return</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>0.000000%</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>调仓后回报率: 首次运行或缺少历史数据</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:32:16</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:32:16</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>2025-05-29_1532:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>position_file</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>pos20250529_v3.csv</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>调仓文件</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:34:23</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>before_trade_balance</t>
+        </is>
+      </c>
+      <c r="B310" t="n">
+        <v>48.07547531</v>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>调仓前账户总保证金余额(totalMarginBalance)</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:34:23</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>before_available_balance</t>
+        </is>
+      </c>
+      <c r="B311" t="n">
+        <v>6.02660723</v>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>调仓前可用保证金余额(available_balance)</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:34:23</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>after_trade_balance</t>
+        </is>
+      </c>
+      <c r="B312" t="n">
+        <v>48.09420452</v>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>调仓后账户总保证金余额(totalMarginBalance)</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:35:37</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>balance_loss</t>
+        </is>
+      </c>
+      <c r="B313" t="n">
+        <v>-0.0187292099999965</v>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>调仓前后账户余额变化</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:35:37</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>balance_loss_rate</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>-0.038958%</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>调仓前后账户余额变化率(%)</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:35:37</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>after_available_balance</t>
+        </is>
+      </c>
+      <c r="B315" t="n">
+        <v>6.06127239</v>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>调仓后可用保证金余额(available_balance)</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:35:37</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>btc_usdt_price</t>
+        </is>
+      </c>
+      <c r="B316" t="n">
+        <v>107879.5</v>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>当前 BTC/USDT 价格: 107879.5</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:35:38</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>trade_commission_summary_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B317" t="n">
+        <v>0</v>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易手续费总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:35:38</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>trade_commission_summary_ratio_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B318" t="n">
+        <v>0</v>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易手续费总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:35:38</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>trade_realized_pnl_summary_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B319" t="n">
+        <v>0</v>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易已实现盈亏总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:35:38</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>trade_realized_pnl_summary_ratio_2025-05-29</t>
+        </is>
+      </c>
+      <c r="B320" t="n">
+        <v>0</v>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>2025-05-29 买卖交易已实现盈亏总和（未计算）</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:35:38</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>pre_rebalance_return</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>0.000000%</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>调仓前回报率: 无历史数据</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:35:37</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>post_rebalance_return</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>0.000000%</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>调仓后回报率: 无历史数据</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>2025-05-29_15:35:37</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>2025-05-29 15:35:38</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>2025-05-29_1534:23</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>